<commit_message>
Updated GTs and eval scripts
</commit_message>
<xml_diff>
--- a/dataset/task_sheet_answers_v2/FutureValue/1_FutureValue/1_FutureValue_gt2.xlsx
+++ b/dataset/task_sheet_answers_v2/FutureValue/1_FutureValue/1_FutureValue_gt2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\MAC\Home\Downloads\workspace\output_dataset_512\70_FutureValue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ActionTransformer\Excel_data\example_sheets_part1\task_sheet_answers_v2\FutureValue\1_FutureValue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8705B7C8-DE6A-4FE9-8D71-C51EADF21EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D925F16-81AB-43A6-97C6-3C890069C5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1380" windowWidth="21600" windowHeight="11333" xr2:uid="{0C7FBAF0-50ED-4A2E-8D68-36C39C8ABDB4}"/>
+    <workbookView xWindow="1980" yWindow="1932" windowWidth="17280" windowHeight="10140" xr2:uid="{0C7FBAF0-50ED-4A2E-8D68-36C39C8ABDB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,10 +62,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,18 +108,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -434,18 +434,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="4" max="4" width="19.46484375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.53125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,7 +486,7 @@
         <v>8503.5955820255986</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -507,7 +507,7 @@
         <v>25575.392591146421</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v>346796.3349208642</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>